<commit_message>
update raw mass sensitivity subplot titles
</commit_message>
<xml_diff>
--- a/Chapter6_Solubility-measurement/data/raw_mass_sensitivity.xlsx
+++ b/Chapter6_Solubility-measurement/data/raw_mass_sensitivity.xlsx
@@ -1,22 +1,22 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="28730"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="29231"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://imperiallondon-my.sharepoint.com/personal/sn621_ic_ac_uk/Documents/Documents/PhD Writings/25-04_PhD Thesis/Chapter6_Sorption/Figures/Python_scripts/data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="19" documentId="11_F25DC773A252ABDACC1048DB599F527C5BDE58E9" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{8B22B654-E7F2-40A5-805D-00B99FDF7AED}"/>
+  <xr:revisionPtr revIDLastSave="23" documentId="11_F25DC773A252ABDACC1048DB599F527C5BDE58E9" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{EE9D91C0-32A6-47EF-AD6C-3B798E53A7C8}"/>
   <bookViews>
-    <workbookView xWindow="2460" yWindow="2589" windowWidth="18514" windowHeight="10740" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="58140" yWindow="-7125" windowWidth="12720" windowHeight="14805" firstSheet="1" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
-    <sheet name="35C_10.0MPa" sheetId="1" r:id="rId1"/>
-    <sheet name="35C_20.1MPa" sheetId="2" r:id="rId2"/>
-    <sheet name="50C_10.1MPa" sheetId="3" r:id="rId3"/>
-    <sheet name="50C_20.1MPa" sheetId="4" r:id="rId4"/>
+    <sheet name="35C_10MPa" sheetId="1" r:id="rId1"/>
+    <sheet name="35C_20MPa" sheetId="2" r:id="rId2"/>
+    <sheet name="50C_10MPa" sheetId="3" r:id="rId3"/>
+    <sheet name="50C_20MPa" sheetId="4" r:id="rId4"/>
   </sheets>
   <calcPr calcId="162913"/>
   <extLst>
@@ -92,10 +92,6 @@
     </ext>
   </extLst>
 </styleSheet>
-</file>
-
-<file path=xl/persons/person.xml><?xml version="1.0" encoding="utf-8"?>
-<personList xmlns="http://schemas.microsoft.com/office/spreadsheetml/2018/threadedcomments" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main"/>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>

</xml_diff>